<commit_message>
filter error in worksheet
</commit_message>
<xml_diff>
--- a/Experiments/Ellipsometry/last-day.xlsx
+++ b/Experiments/Ellipsometry/last-day.xlsx
@@ -2,14 +2,14 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+  <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="18">
   <si>
     <t>MSE = 1.653</t>
   </si>
@@ -71,17 +71,28 @@
   <si>
     <t>thickness</t>
   </si>
+  <si>
+    <t>error</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -110,7 +121,7 @@
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -126,9 +137,9 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="zh-CN"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -166,7 +177,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="zh-CN"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -346,7 +357,7 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-982C-477F-9BBB-B3F21021E813}"/>
             </c:ext>
@@ -360,11 +371,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="235592928"/>
-        <c:axId val="235593256"/>
+        <c:axId val="-709369440"/>
+        <c:axId val="-709366720"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="235592928"/>
+        <c:axId val="-709369440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="60"/>
@@ -419,15 +430,15 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="235593256"/>
+        <c:crossAx val="-709366720"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="235593256"/>
+        <c:axId val="-709366720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -481,10 +492,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="235592928"/>
+        <c:crossAx val="-709369440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -522,7 +533,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="zh-CN"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1094,15 +1105,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>38100</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>41910</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>342900</xdr:colOff>
-      <xdr:row>49</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>118110</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1389,13 +1400,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="W53" sqref="W53"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="O56" sqref="O56"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="20.42578125" customWidth="1"/>
+    <col min="2" max="2" width="20.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:25" x14ac:dyDescent="0.25">
@@ -2674,7 +2685,7 @@
         <v>7.8309999999999994E-3</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>6</v>
       </c>
@@ -2688,7 +2699,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>9</v>
       </c>
@@ -2696,7 +2707,7 @@
         <v>2.7759999999999998</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>10</v>
       </c>
@@ -2707,7 +2718,7 @@
         <v>5.7000000000000002E-2</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>11</v>
       </c>
@@ -2718,7 +2729,7 @@
         <v>7.2028999999999995E-4</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>12</v>
       </c>
@@ -2734,8 +2745,11 @@
       <c r="M38" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N38" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>13</v>
       </c>
@@ -2751,8 +2765,11 @@
       <c r="M39">
         <v>121.63</v>
       </c>
-    </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N39">
+        <v>1.7999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>14</v>
       </c>
@@ -2768,16 +2785,22 @@
       <c r="M40">
         <v>121.78</v>
       </c>
-    </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N40">
+        <v>2.1999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
       <c r="L41">
         <v>80</v>
       </c>
       <c r="M41">
         <v>121.95</v>
       </c>
-    </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N41">
+        <v>1.7999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>6</v>
       </c>
@@ -2796,8 +2819,11 @@
       <c r="M42">
         <v>122.15</v>
       </c>
-    </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N42">
+        <v>2.1000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>9</v>
       </c>
@@ -2810,8 +2836,11 @@
       <c r="M43">
         <v>122.27</v>
       </c>
-    </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N43">
+        <v>2.1999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>10</v>
       </c>
@@ -2827,8 +2856,11 @@
       <c r="M44">
         <v>122.47</v>
       </c>
-    </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N44">
+        <v>3.2000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>11</v>
       </c>
@@ -2844,8 +2876,11 @@
       <c r="M45">
         <v>122.54</v>
       </c>
-    </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N45">
+        <v>2.5999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>12</v>
       </c>
@@ -2861,8 +2896,11 @@
       <c r="M46">
         <v>122.63</v>
       </c>
-    </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N46">
+        <v>2.1999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>13</v>
       </c>
@@ -2878,8 +2916,11 @@
       <c r="M47">
         <v>122.98</v>
       </c>
-    </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N47">
+        <v>3.9E-2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>14</v>
       </c>
@@ -2895,97 +2936,135 @@
       <c r="M48">
         <v>123.09</v>
       </c>
-    </row>
-    <row r="49" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="N48">
+        <v>3.5000000000000003E-2</v>
+      </c>
+    </row>
+    <row r="49" spans="12:14" x14ac:dyDescent="0.25">
       <c r="L49">
         <v>120</v>
       </c>
       <c r="M49">
         <v>123.42</v>
       </c>
-    </row>
-    <row r="50" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="N49">
+        <v>2.9000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="50" spans="12:14" x14ac:dyDescent="0.25">
       <c r="L50">
         <v>125</v>
       </c>
       <c r="M50">
         <v>123.59</v>
       </c>
-    </row>
-    <row r="51" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="N50">
+        <v>3.2000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="51" spans="12:14" x14ac:dyDescent="0.25">
       <c r="L51">
         <v>130</v>
       </c>
       <c r="M51">
         <v>123.98</v>
       </c>
-    </row>
-    <row r="52" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="N51">
+        <v>4.7E-2</v>
+      </c>
+    </row>
+    <row r="52" spans="12:14" x14ac:dyDescent="0.25">
       <c r="L52">
         <v>135</v>
       </c>
       <c r="M52">
         <v>124.45</v>
       </c>
-    </row>
-    <row r="53" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="N52">
+        <v>3.9E-2</v>
+      </c>
+    </row>
+    <row r="53" spans="12:14" x14ac:dyDescent="0.25">
       <c r="L53">
         <v>140</v>
       </c>
       <c r="M53">
         <v>124.88</v>
       </c>
-    </row>
-    <row r="54" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="N53">
+        <v>5.0999999999999997E-2</v>
+      </c>
+    </row>
+    <row r="54" spans="12:14" x14ac:dyDescent="0.25">
       <c r="L54">
         <v>145</v>
       </c>
       <c r="M54">
         <v>125.25</v>
       </c>
-    </row>
-    <row r="55" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="N54">
+        <v>4.9000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="55" spans="12:14" x14ac:dyDescent="0.25">
       <c r="L55">
         <v>150</v>
       </c>
       <c r="M55">
         <v>125.54</v>
       </c>
-    </row>
-    <row r="56" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="N55">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="56" spans="12:14" x14ac:dyDescent="0.25">
       <c r="L56">
         <v>155</v>
       </c>
       <c r="M56">
         <v>125.98</v>
       </c>
-    </row>
-    <row r="57" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="N56">
+        <v>5.5E-2</v>
+      </c>
+    </row>
+    <row r="57" spans="12:14" x14ac:dyDescent="0.25">
       <c r="L57">
         <v>160</v>
       </c>
       <c r="M57">
         <v>126.44</v>
       </c>
-    </row>
-    <row r="58" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="N57">
+        <v>4.3999999999999997E-2</v>
+      </c>
+    </row>
+    <row r="58" spans="12:14" x14ac:dyDescent="0.25">
       <c r="L58">
         <v>165</v>
       </c>
       <c r="M58">
         <v>126.7</v>
       </c>
-    </row>
-    <row r="59" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="N58">
+        <v>5.7000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="59" spans="12:14" x14ac:dyDescent="0.25">
       <c r="L59">
         <v>170</v>
       </c>
       <c r="M59">
         <v>127.1</v>
       </c>
+      <c r="N59">
+        <v>6.0999999999999999E-2</v>
+      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>